<commit_message>
feat：update NPC action change
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/NPCAction_NPC动作表.xlsx
+++ b/dragon-verse/Excels/NPCAction_NPC动作表.xlsx
@@ -1796,7 +1796,7 @@
   <dimension ref="A1:ALY33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9416666666667" defaultRowHeight="16.5"/>
@@ -3272,7 +3272,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="1">
-        <v>132607</v>
+        <v>324757</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
@@ -3297,7 +3297,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="1">
-        <v>132569</v>
+        <v>324754</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -3322,7 +3322,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="1">
-        <v>34419</v>
+        <v>324751</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -3347,7 +3347,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="1">
-        <v>35629</v>
+        <v>324755</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -3372,7 +3372,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="1">
-        <v>35628</v>
+        <v>324758</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
@@ -3397,7 +3397,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="1">
-        <v>35630</v>
+        <v>324761</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
@@ -3422,7 +3422,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="1">
-        <v>34431</v>
+        <v>324753</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
@@ -3447,7 +3447,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="1">
-        <v>35632</v>
+        <v>324759</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
@@ -3472,7 +3472,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="1">
-        <v>34426</v>
+        <v>324756</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -3497,7 +3497,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="1">
-        <v>34417</v>
+        <v>324760</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
@@ -3522,7 +3522,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="1">
-        <v>34430</v>
+        <v>324752</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>

</xml_diff>